<commit_message>
ajout kmeans avec le nv dataset
</commit_message>
<xml_diff>
--- a/kmeans_algo/output/save_metric.xlsx
+++ b/kmeans_algo/output/save_metric.xlsx
@@ -485,25 +485,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.08586043194931559</v>
+        <v>0.06557403506259453</v>
       </c>
       <c r="C2" t="n">
-        <v>0.04206548998333817</v>
+        <v>0.02556334423893891</v>
       </c>
       <c r="D2" t="n">
-        <v>0.04630791023373604</v>
+        <v>0.05288602039217949</v>
       </c>
       <c r="E2" t="n">
-        <v>0.09367820657372807</v>
+        <v>0.132447272676044</v>
       </c>
       <c r="F2" t="n">
-        <v>0.09649321263669604</v>
+        <v>0.133973739915765</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09506487508873357</v>
+        <v>0.1332061333258237</v>
       </c>
       <c r="H2" t="n">
-        <v>0.04515595904686329</v>
+        <v>0.02367381100663764</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -521,25 +521,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5588542279229086</v>
+        <v>0.02015083550910759</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4618147489945009</v>
+        <v>0.006098061199845224</v>
       </c>
       <c r="D3" t="n">
-        <v>0.08005165434200059</v>
+        <v>0.0008833148404090862</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5551681527685928</v>
+        <v>0.05604640154679212</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5716657232281204</v>
+        <v>0.1060689790631738</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5632961704935519</v>
+        <v>0.07334016759995782</v>
       </c>
       <c r="H3" t="n">
-        <v>0.06221621081010732</v>
+        <v>0.009454616866257787</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>

</xml_diff>